<commit_message>
Fixed bug when column changed.
</commit_message>
<xml_diff>
--- a/DM/seed/Focus_Change_Log.xlsx
+++ b/DM/seed/Focus_Change_Log.xlsx
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozenSplit" topLeftCell="E3" xSplit="4" ySplit="2"/>
@@ -1146,6 +1146,74 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="7" t="n">
+        <v>43686</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>D_AGENT,D_OUTLET,D_ADDRESS,D_CUSTOMER,B_AGENT_OWNER</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AddressDetail</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AddressDetailID</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>bigint</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E1:F1"/>

</xml_diff>